<commit_message>
update all results except q2
</commit_message>
<xml_diff>
--- a/pa4_updated/results/results.xlsx
+++ b/pa4_updated/results/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" state="visible" r:id="rId2"/>
@@ -274,12 +274,14 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,7 +316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>15</v>
       </c>
@@ -333,8 +335,17 @@
       <c r="G2" s="0" t="n">
         <v>256</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <v>24.547100067139</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>45.7415580749512</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>195.99461555481</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
@@ -354,8 +365,17 @@
         <f aca="false">G2/2</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="n">
+        <v>23.720741271973</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>56.947808265686</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>277.587652206421</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
@@ -375,8 +395,17 @@
         <f aca="false">G3/2</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="n">
+        <v>24.816989898682</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>373.428087234497</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1520.94984054565</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>15</v>
       </c>
@@ -396,8 +425,17 @@
         <f aca="false">G4/2</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="n">
+        <v>41.059494018555</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>42.305178642273</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>52.809000015259</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
@@ -417,8 +455,17 @@
         <f aca="false">G5/2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="n">
+        <v>25.083780288696</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>492.338185310364</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2013.0443572998</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
@@ -438,8 +485,17 @@
         <f aca="false">G6/2</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="n">
+        <v>84.956884384155</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1333.64731788635</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>3255.2502155304</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>15</v>
       </c>
@@ -459,8 +515,17 @@
         <f aca="false">G7/2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <v>95.087051391602</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1506.9034576416</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>3452.36158370972</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>15</v>
       </c>
@@ -480,8 +545,17 @@
         <f aca="false">G8/2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <v>24.983406066895</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1535.17046928406</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>3254.60505485535</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>15</v>
       </c>
@@ -500,6 +574,15 @@
       <c r="G10" s="0" t="n">
         <f aca="false">G9/2</f>
         <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>143.602132797241</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1707.27368354797</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>3624.65524673462</v>
       </c>
     </row>
   </sheetData>
@@ -520,8 +603,8 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -629,8 +712,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1819,15 +1902,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>16</v>
       </c>
@@ -1881,8 +1966,17 @@
       <c r="G2" s="0" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <v>7.67922401428223</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>991.186089515686</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2669.60167884827</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
@@ -1901,8 +1995,17 @@
       <c r="G3" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="n">
+        <v>835.711240768433</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1782.86859989166</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2810.18853187561</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>16</v>
       </c>
@@ -1921,8 +2024,17 @@
       <c r="G4" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="n">
+        <v>439.357280731201</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1816.2162733078</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>529.885292053223</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
@@ -1941,7 +2053,17 @@
       <c r="G5" s="0" t="n">
         <v>5</v>
       </c>
-    </row>
+      <c r="H5" s="0" t="n">
+        <v>999.941825866699</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1955.56928634644</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>2857.21182823181</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1961,7 +2083,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1998,7 +2120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
@@ -2013,6 +2135,15 @@
       </c>
       <c r="F2" s="0" t="n">
         <v>32</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.091315269470215</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1272.00481891632</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3043.08390617371</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,6 +2163,15 @@
       <c r="F3" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>-0.551700592041016</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>699.028167724609</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>2790.71140289307</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
@@ -2050,8 +2190,17 @@
       <c r="F4" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="n">
+        <v>16.035795211792</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>882.626543045044</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>2444.85831260681</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
@@ -2068,6 +2217,15 @@
       <c r="F5" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <v>0.014258623123169</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>800.652980804443</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>2793.10274124145</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
@@ -2086,6 +2244,15 @@
       <c r="F6" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>9.4149112701416</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1039.55281482023</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>2637.52913475037</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
@@ -2104,6 +2271,15 @@
       <c r="F7" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>4.55832481384277</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>462.775020599365</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1587.60714530945</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
@@ -2122,6 +2298,15 @@
       <c r="F8" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>20.1663970947266</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>859.351439476013</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>2199.44715499878</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
@@ -2140,6 +2325,15 @@
       <c r="F9" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>915.653705596924</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1080.07488250732</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>2534.22617912292</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
@@ -2158,6 +2352,15 @@
       <c r="F10" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>383.78310203552</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1052.47420310974</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>2829.6365737915</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
@@ -2176,6 +2379,15 @@
       <c r="F11" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <v>11.4481449127197</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>952.139973640442</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>2817.60358810425</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
@@ -2194,6 +2406,15 @@
       <c r="F12" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G12" s="0" t="n">
+        <v>296.167850494385</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>714.363503456116</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1865.32354354858</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
@@ -2210,6 +2431,15 @@
       </c>
       <c r="F13" s="0" t="n">
         <v>32</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>311.20777130127</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>2196.19589805603</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>3668.62988471985</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,6 +2459,15 @@
       <c r="F14" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <v>343.307256698608</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>1982.08086490631</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>4415.84420204163</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
@@ -2247,6 +2486,15 @@
       <c r="F15" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <v>75.0269889831543</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1848.61245155334</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>3542.3800945282</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
@@ -2265,6 +2513,15 @@
       <c r="F16" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G16" s="0" t="n">
+        <v>143.241167068481</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>2148.85385036469</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>4374.77207183838</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
@@ -2283,6 +2540,15 @@
       <c r="F17" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G17" s="0" t="n">
+        <v>318.794965744019</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1653.72786334917</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>3501.61790847778</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
@@ -2301,6 +2567,15 @@
       <c r="F18" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G18" s="0" t="n">
+        <v>73.2815265655518</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>871.271386146545</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>2184.43489074707</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
@@ -2319,6 +2594,15 @@
       <c r="F19" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G19" s="0" t="n">
+        <v>457.568168640137</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1975.56987285614</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>3417.7098274231</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
@@ -2337,8 +2621,17 @@
       <c r="F20" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>295.096158981323</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2270.81902503967</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>4357.71441459656</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>15</v>
       </c>
@@ -2355,6 +2648,15 @@
       <c r="F21" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G21" s="0" t="n">
+        <v>981.707811355591</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>2247.68191814423</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>5766.39747619629</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
@@ -2373,6 +2675,15 @@
       <c r="F22" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="G22" s="0" t="n">
+        <v>364.18080329895</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1919.61618900299</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>4540.67158699036</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
@@ -2390,6 +2701,15 @@
       </c>
       <c r="F23" s="0" t="n">
         <v>32</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>1266.26014709473</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>1716.67952060699</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>3529.95371818542</v>
       </c>
     </row>
   </sheetData>
@@ -2411,12 +2731,15 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>16</v>
       </c>
@@ -2470,8 +2793,17 @@
       <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <v>22.1805572509766</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1562.84219741821</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2929.05449867249</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
@@ -2491,8 +2823,17 @@
       <c r="G3" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="n">
+        <v>383.237361907959</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1594.47516441345</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2596.84538841248</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>16</v>
       </c>
@@ -2512,8 +2853,17 @@
       <c r="G4" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="n">
+        <v>325.848579406738</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1689.62530136108</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>2817.92712211609</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
@@ -2533,8 +2883,17 @@
       <c r="G5" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="n">
+        <v>13.9522552490234</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>598.256940841675</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>2378.63111495972</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>16</v>
       </c>
@@ -2554,8 +2913,17 @@
       <c r="G6" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="n">
+        <v>259.003162384033</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1285.35953044891</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2708.88090133667</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
@@ -2575,8 +2943,17 @@
       <c r="G7" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="n">
+        <v>343.365430831909</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1390.90505599976</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>2705.19375801086</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>16</v>
       </c>
@@ -2596,8 +2973,17 @@
       <c r="G8" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <v>30.4057598114014</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>557.942199707031</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>2319.46277618408</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>16</v>
       </c>
@@ -2617,8 +3003,17 @@
       <c r="G9" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <v>984.304904937744</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1655.45372962952</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>2450.71697235107</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>16</v>
       </c>
@@ -2638,8 +3033,17 @@
       <c r="G10" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <v>433.937311172485</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1611.06032848358</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>2745.79954147339</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>16</v>
       </c>
@@ -2659,8 +3063,17 @@
       <c r="G11" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="n">
+        <v>55.1207065582275</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>480.279841423035</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1064.91279602051</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>16</v>
       </c>
@@ -2679,6 +3092,15 @@
       </c>
       <c r="G12" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>140.529870986938</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1081.06266498566</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>2312.04295158386</v>
       </c>
     </row>
   </sheetData>
@@ -2697,10 +3119,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2737,7 +3159,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
@@ -2753,8 +3175,20 @@
       <c r="F2" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
@@ -2771,8 +3205,20 @@
       <c r="F3" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
@@ -2789,8 +3235,20 @@
       <c r="F4" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
@@ -2807,8 +3265,20 @@
       <c r="F5" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
@@ -2825,8 +3295,20 @@
       <c r="F6" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
@@ -2843,8 +3325,20 @@
       <c r="F7" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
@@ -2861,8 +3355,20 @@
       <c r="F8" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>14</v>
       </c>
@@ -2879,8 +3385,20 @@
       <c r="F9" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>14</v>
       </c>
@@ -2897,8 +3415,20 @@
       <c r="F10" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>14</v>
       </c>
@@ -2915,8 +3445,20 @@
       <c r="F11" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>14</v>
       </c>
@@ -2933,8 +3475,20 @@
       <c r="F12" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>15</v>
       </c>
@@ -2950,8 +3504,20 @@
       <c r="F13" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>15</v>
       </c>
@@ -2968,8 +3534,20 @@
       <c r="F14" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>15</v>
       </c>
@@ -2986,8 +3564,20 @@
       <c r="F15" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>15</v>
       </c>
@@ -3004,8 +3594,20 @@
       <c r="F16" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>15</v>
       </c>
@@ -3022,8 +3624,20 @@
       <c r="F17" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>15</v>
       </c>
@@ -3040,8 +3654,20 @@
       <c r="F18" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>15</v>
       </c>
@@ -3058,8 +3684,20 @@
       <c r="F19" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>15</v>
       </c>
@@ -3076,8 +3714,20 @@
       <c r="F20" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>15</v>
       </c>
@@ -3094,8 +3744,20 @@
       <c r="F21" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>15</v>
       </c>
@@ -3112,8 +3774,20 @@
       <c r="F22" s="0" t="n">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>15</v>
       </c>
@@ -3129,6 +3803,18 @@
       </c>
       <c r="F23" s="0" t="n">
         <v>32</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3147,10 +3833,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3190,7 +3876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>16</v>
       </c>
@@ -3209,8 +3895,20 @@
       <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
@@ -3230,8 +3928,20 @@
       <c r="G3" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>16</v>
       </c>
@@ -3251,8 +3961,20 @@
       <c r="G4" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
@@ -3272,8 +3994,20 @@
       <c r="G5" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>16</v>
       </c>
@@ -3293,8 +4027,20 @@
       <c r="G6" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
@@ -3314,8 +4060,20 @@
       <c r="G7" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>16</v>
       </c>
@@ -3335,8 +4093,20 @@
       <c r="G8" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>16</v>
       </c>
@@ -3356,8 +4126,20 @@
       <c r="G9" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>16</v>
       </c>
@@ -3377,8 +4159,20 @@
       <c r="G10" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>16</v>
       </c>
@@ -3398,8 +4192,20 @@
       <c r="G11" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>16</v>
       </c>
@@ -3418,6 +4224,18 @@
       </c>
       <c r="G12" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3439,7 +4257,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3470,7 +4288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
@@ -3486,8 +4304,11 @@
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="0" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
@@ -3504,8 +4325,11 @@
         <f aca="false">F2*2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
@@ -3522,8 +4346,11 @@
         <f aca="false">F3*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>14</v>
       </c>
@@ -3540,8 +4367,11 @@
         <f aca="false">F4*2</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
@@ -3558,8 +4388,11 @@
         <f aca="false">F5*2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
@@ -3576,8 +4409,11 @@
         <f aca="false">F6*2</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="0" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
@@ -3594,8 +4430,11 @@
         <f aca="false">F7*2</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="0" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>14</v>
       </c>
@@ -3612,8 +4451,11 @@
         <f aca="false">F8*2</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>14</v>
       </c>
@@ -3630,8 +4472,11 @@
         <f aca="false">F9*2</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>14</v>
       </c>
@@ -3648,8 +4493,11 @@
         <f aca="false">F10*2</f>
         <v>512</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>14</v>
       </c>
@@ -3666,8 +4514,11 @@
         <f aca="false">F11*2</f>
         <v>1024</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="0" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>14</v>
       </c>
@@ -3684,8 +4535,11 @@
         <f aca="false">F12*2</f>
         <v>2048</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="n">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>14</v>
       </c>
@@ -3702,8 +4556,11 @@
         <f aca="false">F13*2</f>
         <v>4096</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="n">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>14</v>
       </c>
@@ -3720,8 +4577,11 @@
         <f aca="false">F14*2</f>
         <v>8192</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="0" t="n">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>14</v>
       </c>
@@ -3738,8 +4598,11 @@
         <f aca="false">F15*2</f>
         <v>16384</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="n">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>14</v>
       </c>
@@ -3756,8 +4619,11 @@
         <f aca="false">F16*2</f>
         <v>32768</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="n">
+        <v>4092</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>14</v>
       </c>
@@ -3774,8 +4640,11 @@
         <f aca="false">F17*2</f>
         <v>65536</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="n">
+        <v>8184</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>14</v>
       </c>
@@ -3792,8 +4661,11 @@
         <f aca="false">F18*2</f>
         <v>131072</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="n">
+        <v>16368</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>14</v>
       </c>
@@ -3810,8 +4682,11 @@
         <f aca="false">F19*2</f>
         <v>262144</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>32550</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>14</v>
       </c>
@@ -3828,8 +4703,11 @@
         <f aca="false">F20*2</f>
         <v>524288</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="n">
+        <v>65100</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>14</v>
       </c>
@@ -3845,6 +4723,9 @@
       <c r="F22" s="0" t="n">
         <f aca="false">F21*2</f>
         <v>1048576</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>130200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>